<commit_message>
Sympy using real data
</commit_message>
<xml_diff>
--- a/ManualDataManipulation/Example_Data_TE11764.xlsx
+++ b/ManualDataManipulation/Example_Data_TE11764.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/mter153_uoa_auckland_ac_nz/Documents/P4P/p4p-geothermalML/ManualDataManipulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University_Materials\2024\P4P\p4p-geothermalML\ManualDataManipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5386E6D-D00B-4E03-B049-0BFD040DCE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAD0D5D-F529-4A98-B129-71991EAF75AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -2484,7 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>

</xml_diff>